<commit_message>
included the logic for listing trades
</commit_message>
<xml_diff>
--- a/dhan_excel/DhanTrading.xlsx
+++ b/dhan_excel/DhanTrading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AlgoTrading\Books\Sucessful Algorithmic Trading\SucessfulAlgoTrading\dhan_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E6C94D-4A6E-4CC4-B8B0-0975A4E0B9E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084A01A7-08D6-4377-AAF7-0F0421B5341A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3F6F1494-9B09-4F57-8AEB-2BA84EF373A6}"/>
   </bookViews>
@@ -16,11 +16,13 @@
     <sheet name="Trade" sheetId="1" r:id="rId1"/>
     <sheet name="OptionsLookUp" sheetId="2" r:id="rId2"/>
     <sheet name="IndexLookup" sheetId="3" r:id="rId3"/>
+    <sheet name="Orders" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">OptionsLookUp!$A$1:$B$1257</definedName>
     <definedName name="ATM_KEY">Trade!$G$6</definedName>
     <definedName name="ATM_LTP">Trade!$H$6</definedName>
+    <definedName name="Generate_PL">Trade!$B$31</definedName>
     <definedName name="INDEX_LTP">Trade!$B$3</definedName>
     <definedName name="IndexKey">Trade!$B$25</definedName>
     <definedName name="INSTRUMENT">Trade!$B$23</definedName>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1332" uniqueCount="1313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1664" uniqueCount="1355">
   <si>
     <t>Instrument</t>
   </si>
@@ -3980,7 +3982,133 @@
     <t>Refresh</t>
   </si>
   <si>
-    <t>NIFTY CE</t>
+    <t>Generate PL</t>
+  </si>
+  <si>
+    <t>CRUDEOIL PE</t>
+  </si>
+  <si>
+    <t>dhanClientId</t>
+  </si>
+  <si>
+    <t>orderId</t>
+  </si>
+  <si>
+    <t>exchangeOrderId</t>
+  </si>
+  <si>
+    <t>exchangeTradeId</t>
+  </si>
+  <si>
+    <t>transactionType</t>
+  </si>
+  <si>
+    <t>exchangeSegment</t>
+  </si>
+  <si>
+    <t>productType</t>
+  </si>
+  <si>
+    <t>orderType</t>
+  </si>
+  <si>
+    <t>tradingSymbol</t>
+  </si>
+  <si>
+    <t>customSymbol</t>
+  </si>
+  <si>
+    <t>securityId</t>
+  </si>
+  <si>
+    <t>tradedQuantity</t>
+  </si>
+  <si>
+    <t>tradedPrice</t>
+  </si>
+  <si>
+    <t>createTime</t>
+  </si>
+  <si>
+    <t>updateTime</t>
+  </si>
+  <si>
+    <t>exchangeTime</t>
+  </si>
+  <si>
+    <t>drvExpiryDate</t>
+  </si>
+  <si>
+    <t>drvOptionType</t>
+  </si>
+  <si>
+    <t>drvStrikePrice</t>
+  </si>
+  <si>
+    <t>BUY</t>
+  </si>
+  <si>
+    <t>NSE_EQ</t>
+  </si>
+  <si>
+    <t>CNC</t>
+  </si>
+  <si>
+    <t>MARKET</t>
+  </si>
+  <si>
+    <t>OLAELEC</t>
+  </si>
+  <si>
+    <t>0001-01-01</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>SELL</t>
+  </si>
+  <si>
+    <t>NSE_FNO</t>
+  </si>
+  <si>
+    <t>INTRADAY</t>
+  </si>
+  <si>
+    <t>LIMIT</t>
+  </si>
+  <si>
+    <t>NIFTY-Dec2024-23750-PE</t>
+  </si>
+  <si>
+    <t>NIFTY-Dec2024-23600-CE</t>
+  </si>
+  <si>
+    <t>NIFTY-Dec2024-23850-PE</t>
+  </si>
+  <si>
+    <t>NIFTY-Dec2024-23750-CE</t>
+  </si>
+  <si>
+    <t>NIFTY-Dec2024-FUT</t>
+  </si>
+  <si>
+    <t>BANKNIFTY-Jan2025-51300-CE</t>
+  </si>
+  <si>
+    <t>NIFTY-Dec2024-23900-PE</t>
+  </si>
+  <si>
+    <t>NIFTY-Dec2024-23800-CE</t>
+  </si>
+  <si>
+    <t>CRUDEOIL-15Jan2025-5900-CE</t>
+  </si>
+  <si>
+    <t>CRUDEOIL-15Jan2025-5950-PE</t>
+  </si>
+  <si>
+    <t>CRUDEOIL-15Jan2025-6000-PE</t>
   </si>
 </sst>
 </file>
@@ -4030,7 +4158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -4042,6 +4170,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4356,11 +4486,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F7CD468-4C8C-49F2-898A-9AFC5D722CAC}">
-  <dimension ref="A1:Y29"/>
+  <dimension ref="A1:Y31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="12" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y14" sqref="Y14"/>
+      <pane xSplit="12" topLeftCell="R1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4371,14 +4501,14 @@
     <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="22.5703125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="10.5703125" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" customWidth="1"/>
+    <col min="16" max="16" width="22.5703125" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" customWidth="1"/>
+    <col min="18" max="18" width="10.5703125" customWidth="1"/>
     <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="16.5703125" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="19.42578125" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="18" customWidth="1"/>
+    <col min="21" max="21" width="16.5703125" customWidth="1"/>
+    <col min="22" max="22" width="19.42578125" customWidth="1"/>
     <col min="23" max="23" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -4395,7 +4525,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -4403,7 +4533,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>23803.45</v>
+        <v>5943</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -4482,7 +4612,7 @@
       </c>
       <c r="B5" s="3">
         <f>IF(LEFT(B2,1)="N",25,IF(LEFT(B2,1)="B",15,IF(LEFT(B2,1)="C",100,"")))</f>
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>25</v>
@@ -4554,18 +4684,18 @@
       </c>
       <c r="E6">
         <f>$B$3-MOD($B$3,$B$4)</f>
-        <v>23800</v>
+        <v>5900</v>
       </c>
       <c r="F6" t="str">
         <f>$B$22&amp;"_"&amp;E6</f>
-        <v>NIFTY_CE_23800</v>
+        <v>CRUDEOIL_PE_5900</v>
       </c>
       <c r="G6">
         <f>VLOOKUP(F6,OptionsLookUp!A:B,2,FALSE)</f>
-        <v>41687</v>
+        <v>441308</v>
       </c>
       <c r="H6">
-        <v>79.45</v>
+        <v>144.19999999999999</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>IF(I6&lt;&gt;"",ROUNDDOWN($B$7*(IF(AND(I6&gt;0,I6&lt;10),I6/10,1))/H6/$B$5,0)*$B$27,"")</f>
@@ -4600,25 +4730,25 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
       </c>
       <c r="E7">
         <f>IF($B$24="PE",$E$6+($B$4*RIGHT(D7,1)),$E$6-($B$4*RIGHT(D7,1)))</f>
-        <v>23750</v>
+        <v>5950</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" ref="F7:F9" si="1">$B$22&amp;"_"&amp;E7</f>
-        <v>NIFTY_CE_23750</v>
+        <v>CRUDEOIL_PE_5950</v>
       </c>
       <c r="G7">
         <f>VLOOKUP(F7,OptionsLookUp!A:B,2,FALSE)</f>
-        <v>41685</v>
+        <v>441392</v>
       </c>
       <c r="H7">
-        <v>112.25</v>
+        <v>168.4</v>
       </c>
       <c r="J7" s="3" t="str">
         <f t="shared" ref="J7:J9" si="2">IF(I7&lt;&gt;"",ROUNDDOWN($B$7*(IF(AND(I7&gt;0,I7&lt;10),I7/10,1))/H7/$B$5,0)*$B$27,"")</f>
@@ -4653,25 +4783,25 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="D8" t="s">
         <v>23</v>
       </c>
       <c r="E8">
         <f>IF($B$24="PE",$E$6+($B$4*RIGHT(D8,1)),$E$6-($B$4*RIGHT(D8,1)))</f>
-        <v>23700</v>
+        <v>6000</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="1"/>
-        <v>NIFTY_CE_23700</v>
+        <v>CRUDEOIL_PE_6000</v>
       </c>
       <c r="G8">
         <f>VLOOKUP(F8,OptionsLookUp!A:B,2,FALSE)</f>
-        <v>41683</v>
+        <v>441393</v>
       </c>
       <c r="H8">
-        <v>150.30000000000001</v>
+        <v>194.3</v>
       </c>
       <c r="J8" s="3" t="str">
         <f t="shared" si="2"/>
@@ -4706,25 +4836,25 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="D9" t="s">
         <v>24</v>
       </c>
       <c r="E9">
         <f>IF($B$24="PE",$E$6+($B$4*RIGHT(D9,1)),$E$6-($B$4*RIGHT(D9,1)))</f>
-        <v>23650</v>
+        <v>6050</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="1"/>
-        <v>NIFTY_CE_23650</v>
+        <v>CRUDEOIL_PE_6050</v>
       </c>
       <c r="G9">
         <f>VLOOKUP(F9,OptionsLookUp!A:B,2,FALSE)</f>
-        <v>41681</v>
+        <v>441394</v>
       </c>
       <c r="H9">
-        <v>191.85</v>
+        <v>221.8</v>
       </c>
       <c r="J9" s="3" t="str">
         <f t="shared" si="2"/>
@@ -4760,7 +4890,7 @@
       </c>
       <c r="B10" s="2">
         <f>B8-B9</f>
-        <v>3.0000000000000002E-2</v>
+        <v>1.9999999999999997E-2</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -4795,7 +4925,7 @@
       </c>
       <c r="B17">
         <f>B13*B10</f>
-        <v>3.0000000000000002E-2</v>
+        <v>1.9999999999999997E-2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -4804,7 +4934,7 @@
       </c>
       <c r="B18">
         <f>B14*B10</f>
-        <v>3.0000000000000002E-2</v>
+        <v>1.9999999999999997E-2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -4813,7 +4943,7 @@
       </c>
       <c r="B19">
         <f>B13*B8</f>
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -4822,7 +4952,7 @@
       </c>
       <c r="B20">
         <f>B14*B8</f>
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -4831,7 +4961,7 @@
       </c>
       <c r="B22" t="str">
         <f>B23&amp;"_"&amp;B24</f>
-        <v>NIFTY_CE</v>
+        <v>CRUDEOIL_PE</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -4840,7 +4970,7 @@
       </c>
       <c r="B23" t="str">
         <f>LEFT(B2,FIND(" ",B2,1)-1)</f>
-        <v>NIFTY</v>
+        <v>CRUDEOIL</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -4849,7 +4979,7 @@
       </c>
       <c r="B24" t="str">
         <f>RIGHT(B2,2)</f>
-        <v>CE</v>
+        <v>PE</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -4858,7 +4988,7 @@
       </c>
       <c r="B25">
         <f>VLOOKUP(B23,IndexLookup!A1:B4,2,FALSE)</f>
-        <v>13</v>
+        <v>436953</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -4867,7 +4997,7 @@
       </c>
       <c r="B27">
         <f>IF(OR(LEFT(B2,1)="N",LEFT(B2,1)="B"),B5,1)</f>
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -4875,6 +5005,14 @@
         <v>1311</v>
       </c>
       <c r="B29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B31" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4882,12 +5020,15 @@
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{069EE39A-D232-48A5-A4AA-01A48D494282}">
       <formula1>"NIFTY PE, NIFTY CE, BANKNIFTY PE, BANKNIFTY CE,CRUDEOIL CE, CRUDEOIL PE"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B29" xr:uid="{A1FEE6D5-54C4-461C-B04B-7F0563CB22A3}">
       <formula1>"True, False"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31" xr:uid="{AABBCC32-78FC-4E10-AEEC-401979DA1033}">
+      <formula1>"FALSE,TRUE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15019,4 +15160,3041 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEE9CD5B-D3BC-4F86-A24A-79774DBFB8C1}">
+  <dimension ref="A1:S54"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1315</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1316</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1317</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1318</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1320</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1321</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1322</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1323</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1324</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1325</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1326</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1327</v>
+      </c>
+      <c r="O1" t="s">
+        <v>1328</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1329</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="R1" t="s">
+        <v>1331</v>
+      </c>
+      <c r="S1" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1100381471</v>
+      </c>
+      <c r="B2">
+        <v>10124122424093</v>
+      </c>
+      <c r="C2">
+        <v>1200000024877180</v>
+      </c>
+      <c r="D2">
+        <v>402814470</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1334</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1335</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1336</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1337</v>
+      </c>
+      <c r="K2">
+        <v>24777</v>
+      </c>
+      <c r="L2">
+        <v>3</v>
+      </c>
+      <c r="M2">
+        <v>94.22</v>
+      </c>
+      <c r="N2" s="7">
+        <v>45650.466238425928</v>
+      </c>
+      <c r="O2" s="7">
+        <v>45650.466238425928</v>
+      </c>
+      <c r="P2" s="7">
+        <v>45650.466238425928</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>1338</v>
+      </c>
+      <c r="R2" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1100381471</v>
+      </c>
+      <c r="B3">
+        <v>10124122424093</v>
+      </c>
+      <c r="C3">
+        <v>1200000024877180</v>
+      </c>
+      <c r="D3">
+        <v>402814471</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1335</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1336</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1337</v>
+      </c>
+      <c r="K3">
+        <v>24777</v>
+      </c>
+      <c r="L3">
+        <v>8</v>
+      </c>
+      <c r="M3">
+        <v>94.23</v>
+      </c>
+      <c r="N3" s="7">
+        <v>45650.466238425928</v>
+      </c>
+      <c r="O3" s="7">
+        <v>45650.466238425928</v>
+      </c>
+      <c r="P3" s="7">
+        <v>45650.466238425928</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>1338</v>
+      </c>
+      <c r="R3" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1100381471</v>
+      </c>
+      <c r="B4">
+        <v>1224122462316</v>
+      </c>
+      <c r="C4">
+        <v>1100000009423060</v>
+      </c>
+      <c r="D4">
+        <v>429155</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1344</v>
+      </c>
+      <c r="K4">
+        <v>41686</v>
+      </c>
+      <c r="L4">
+        <v>50</v>
+      </c>
+      <c r="M4">
+        <v>97.8</v>
+      </c>
+      <c r="N4" s="7">
+        <v>45650.397824074076</v>
+      </c>
+      <c r="O4" s="7">
+        <v>45650.397824074076</v>
+      </c>
+      <c r="P4" s="7">
+        <v>45650.397824074076</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R4" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S4">
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1100381471</v>
+      </c>
+      <c r="B5">
+        <v>1224122462316</v>
+      </c>
+      <c r="C5">
+        <v>1100000009423060</v>
+      </c>
+      <c r="D5">
+        <v>429156</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1340</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1344</v>
+      </c>
+      <c r="K5">
+        <v>41686</v>
+      </c>
+      <c r="L5">
+        <v>50</v>
+      </c>
+      <c r="M5">
+        <v>97.8</v>
+      </c>
+      <c r="N5" s="7">
+        <v>45650.397824074076</v>
+      </c>
+      <c r="O5" s="7">
+        <v>45650.397824074076</v>
+      </c>
+      <c r="P5" s="7">
+        <v>45650.397824074076</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R5" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S5">
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1100381471</v>
+      </c>
+      <c r="B6">
+        <v>2224122454316</v>
+      </c>
+      <c r="C6">
+        <v>1400000009586320</v>
+      </c>
+      <c r="D6">
+        <v>335764</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1336</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1345</v>
+      </c>
+      <c r="K6">
+        <v>41672</v>
+      </c>
+      <c r="L6">
+        <v>25</v>
+      </c>
+      <c r="M6">
+        <v>206.45</v>
+      </c>
+      <c r="N6" s="7">
+        <v>45650.395937499998</v>
+      </c>
+      <c r="O6" s="7">
+        <v>45650.395937499998</v>
+      </c>
+      <c r="P6" s="7">
+        <v>45650.395937499998</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S6">
+        <v>23600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1100381471</v>
+      </c>
+      <c r="B7">
+        <v>2224122459716</v>
+      </c>
+      <c r="C7">
+        <v>1400000010670190</v>
+      </c>
+      <c r="D7">
+        <v>367383</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1336</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1345</v>
+      </c>
+      <c r="K7">
+        <v>41672</v>
+      </c>
+      <c r="L7">
+        <v>25</v>
+      </c>
+      <c r="M7">
+        <v>193.95</v>
+      </c>
+      <c r="N7" s="7">
+        <v>45650.397106481483</v>
+      </c>
+      <c r="O7" s="7">
+        <v>45650.397106481483</v>
+      </c>
+      <c r="P7" s="7">
+        <v>45650.397106481483</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R7" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S7">
+        <v>23600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1100381471</v>
+      </c>
+      <c r="B8">
+        <v>4224122473016</v>
+      </c>
+      <c r="C8">
+        <v>1100000009269250</v>
+      </c>
+      <c r="D8">
+        <v>425266</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1344</v>
+      </c>
+      <c r="K8">
+        <v>41686</v>
+      </c>
+      <c r="L8">
+        <v>50</v>
+      </c>
+      <c r="M8">
+        <v>93.1</v>
+      </c>
+      <c r="N8" s="7">
+        <v>45650.39775462963</v>
+      </c>
+      <c r="O8" s="7">
+        <v>45650.39775462963</v>
+      </c>
+      <c r="P8" s="7">
+        <v>45650.39775462963</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R8" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S8">
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1100381471</v>
+      </c>
+      <c r="B9">
+        <v>4224122473016</v>
+      </c>
+      <c r="C9">
+        <v>1100000009269250</v>
+      </c>
+      <c r="D9">
+        <v>425272</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1344</v>
+      </c>
+      <c r="K9">
+        <v>41686</v>
+      </c>
+      <c r="L9">
+        <v>25</v>
+      </c>
+      <c r="M9">
+        <v>93.1</v>
+      </c>
+      <c r="N9" s="7">
+        <v>45650.39775462963</v>
+      </c>
+      <c r="O9" s="7">
+        <v>45650.39775462963</v>
+      </c>
+      <c r="P9" s="7">
+        <v>45650.39775462963</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R9" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S9">
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1100381471</v>
+      </c>
+      <c r="B10">
+        <v>4224122473016</v>
+      </c>
+      <c r="C10">
+        <v>1100000009269250</v>
+      </c>
+      <c r="D10">
+        <v>425273</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H10" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1344</v>
+      </c>
+      <c r="K10">
+        <v>41686</v>
+      </c>
+      <c r="L10">
+        <v>25</v>
+      </c>
+      <c r="M10">
+        <v>93.1</v>
+      </c>
+      <c r="N10" s="7">
+        <v>45650.39775462963</v>
+      </c>
+      <c r="O10" s="7">
+        <v>45650.39775462963</v>
+      </c>
+      <c r="P10" s="7">
+        <v>45650.39775462963</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R10" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S10">
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1100381471</v>
+      </c>
+      <c r="B11">
+        <v>12241224174116</v>
+      </c>
+      <c r="C11">
+        <v>1300000027523850</v>
+      </c>
+      <c r="D11">
+        <v>649684</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1340</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H11" t="s">
+        <v>1336</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1346</v>
+      </c>
+      <c r="K11">
+        <v>41690</v>
+      </c>
+      <c r="L11">
+        <v>25</v>
+      </c>
+      <c r="M11">
+        <v>102.35</v>
+      </c>
+      <c r="N11" s="7">
+        <v>45650.421111111114</v>
+      </c>
+      <c r="O11" s="7">
+        <v>45650.421111111114</v>
+      </c>
+      <c r="P11" s="7">
+        <v>45650.421111111114</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R11" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S11">
+        <v>23850</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1100381471</v>
+      </c>
+      <c r="B12">
+        <v>12241224308016</v>
+      </c>
+      <c r="C12">
+        <v>1100000056041810</v>
+      </c>
+      <c r="D12">
+        <v>1795570</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H12" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1347</v>
+      </c>
+      <c r="K12">
+        <v>41685</v>
+      </c>
+      <c r="L12">
+        <v>25</v>
+      </c>
+      <c r="M12">
+        <v>154.35</v>
+      </c>
+      <c r="N12" s="7">
+        <v>45650.462789351855</v>
+      </c>
+      <c r="O12" s="7">
+        <v>45650.462789351855</v>
+      </c>
+      <c r="P12" s="7">
+        <v>45650.462789351855</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R12" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S12">
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1100381471</v>
+      </c>
+      <c r="B13">
+        <v>12241224364416</v>
+      </c>
+      <c r="C13">
+        <v>1100000068068820</v>
+      </c>
+      <c r="D13">
+        <v>1984248</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1340</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H13" t="s">
+        <v>1336</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1347</v>
+      </c>
+      <c r="K13">
+        <v>41685</v>
+      </c>
+      <c r="L13">
+        <v>25</v>
+      </c>
+      <c r="M13">
+        <v>149.4</v>
+      </c>
+      <c r="N13" s="7">
+        <v>45650.49082175926</v>
+      </c>
+      <c r="O13" s="7">
+        <v>45650.49082175926</v>
+      </c>
+      <c r="P13" s="7">
+        <v>45650.49082175926</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R13" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S13">
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1100381471</v>
+      </c>
+      <c r="B14">
+        <v>12241224385016</v>
+      </c>
+      <c r="C14">
+        <v>1000000107173810</v>
+      </c>
+      <c r="D14">
+        <v>3268048</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1340</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H14" t="s">
+        <v>1336</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1348</v>
+      </c>
+      <c r="K14">
+        <v>35005</v>
+      </c>
+      <c r="L14">
+        <v>25</v>
+      </c>
+      <c r="M14">
+        <v>23820.5</v>
+      </c>
+      <c r="N14" s="7">
+        <v>45650.503460648149</v>
+      </c>
+      <c r="O14" s="7">
+        <v>45650.503460648149</v>
+      </c>
+      <c r="P14" s="7">
+        <v>45650.503460648149</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R14" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S14">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1100381471</v>
+      </c>
+      <c r="B15">
+        <v>12241224395616</v>
+      </c>
+      <c r="C15">
+        <v>1300000077651870</v>
+      </c>
+      <c r="D15">
+        <v>2128375</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H15" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I15" t="s">
+        <v>1346</v>
+      </c>
+      <c r="K15">
+        <v>41690</v>
+      </c>
+      <c r="L15">
+        <v>25</v>
+      </c>
+      <c r="M15">
+        <v>96.85</v>
+      </c>
+      <c r="N15" s="7">
+        <v>45650.508032407408</v>
+      </c>
+      <c r="O15" s="7">
+        <v>45650.508032407408</v>
+      </c>
+      <c r="P15" s="7">
+        <v>45650.508032407408</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R15" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S15">
+        <v>23850</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1100381471</v>
+      </c>
+      <c r="B16">
+        <v>12241224450816</v>
+      </c>
+      <c r="C16">
+        <v>1300000091365380</v>
+      </c>
+      <c r="D16">
+        <v>2471941</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1340</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H16" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I16" t="s">
+        <v>1346</v>
+      </c>
+      <c r="K16">
+        <v>41690</v>
+      </c>
+      <c r="L16">
+        <v>25</v>
+      </c>
+      <c r="M16">
+        <v>82.1</v>
+      </c>
+      <c r="N16" s="7">
+        <v>45650.531747685185</v>
+      </c>
+      <c r="O16" s="7">
+        <v>45650.531747685185</v>
+      </c>
+      <c r="P16" s="7">
+        <v>45650.531747685185</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R16" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S16">
+        <v>23850</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1100381471</v>
+      </c>
+      <c r="B17">
+        <v>12241224542216</v>
+      </c>
+      <c r="C17">
+        <v>1300000116321080</v>
+      </c>
+      <c r="D17">
+        <v>3032486</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H17" t="s">
+        <v>1336</v>
+      </c>
+      <c r="I17" t="s">
+        <v>1346</v>
+      </c>
+      <c r="K17">
+        <v>41690</v>
+      </c>
+      <c r="L17">
+        <v>50</v>
+      </c>
+      <c r="M17">
+        <v>123.45</v>
+      </c>
+      <c r="N17" s="7">
+        <v>45650.584467592591</v>
+      </c>
+      <c r="O17" s="7">
+        <v>45650.584467592591</v>
+      </c>
+      <c r="P17" s="7">
+        <v>45650.584467592591</v>
+      </c>
+      <c r="Q17" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R17" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S17">
+        <v>23850</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1100381471</v>
+      </c>
+      <c r="B18">
+        <v>12241224542216</v>
+      </c>
+      <c r="C18">
+        <v>1300000116321080</v>
+      </c>
+      <c r="D18">
+        <v>3032487</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H18" t="s">
+        <v>1336</v>
+      </c>
+      <c r="I18" t="s">
+        <v>1346</v>
+      </c>
+      <c r="K18">
+        <v>41690</v>
+      </c>
+      <c r="L18">
+        <v>25</v>
+      </c>
+      <c r="M18">
+        <v>123.45</v>
+      </c>
+      <c r="N18" s="7">
+        <v>45650.584467592591</v>
+      </c>
+      <c r="O18" s="7">
+        <v>45650.584467592591</v>
+      </c>
+      <c r="P18" s="7">
+        <v>45650.584467592591</v>
+      </c>
+      <c r="Q18" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R18" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S18">
+        <v>23850</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1100381471</v>
+      </c>
+      <c r="B19">
+        <v>12241224548316</v>
+      </c>
+      <c r="C19">
+        <v>1300000117884340</v>
+      </c>
+      <c r="D19">
+        <v>3074748</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1340</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H19" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I19" t="s">
+        <v>1346</v>
+      </c>
+      <c r="K19">
+        <v>41690</v>
+      </c>
+      <c r="L19">
+        <v>25</v>
+      </c>
+      <c r="M19">
+        <v>134.94999999999999</v>
+      </c>
+      <c r="N19" s="7">
+        <v>45650.589108796295</v>
+      </c>
+      <c r="O19" s="7">
+        <v>45650.589108796295</v>
+      </c>
+      <c r="P19" s="7">
+        <v>45650.589108796295</v>
+      </c>
+      <c r="Q19" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R19" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S19">
+        <v>23850</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1100381471</v>
+      </c>
+      <c r="B20">
+        <v>12241224548316</v>
+      </c>
+      <c r="C20">
+        <v>1300000117884340</v>
+      </c>
+      <c r="D20">
+        <v>3074749</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1340</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G20" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H20" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I20" t="s">
+        <v>1346</v>
+      </c>
+      <c r="K20">
+        <v>41690</v>
+      </c>
+      <c r="L20">
+        <v>50</v>
+      </c>
+      <c r="M20">
+        <v>134.94999999999999</v>
+      </c>
+      <c r="N20" s="7">
+        <v>45650.589108796295</v>
+      </c>
+      <c r="O20" s="7">
+        <v>45650.589108796295</v>
+      </c>
+      <c r="P20" s="7">
+        <v>45650.589108796295</v>
+      </c>
+      <c r="Q20" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R20" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S20">
+        <v>23850</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1100381471</v>
+      </c>
+      <c r="B21">
+        <v>22241224380616</v>
+      </c>
+      <c r="C21">
+        <v>1300000072429540</v>
+      </c>
+      <c r="D21">
+        <v>1954727</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H21" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I21" t="s">
+        <v>1346</v>
+      </c>
+      <c r="K21">
+        <v>41690</v>
+      </c>
+      <c r="L21">
+        <v>50</v>
+      </c>
+      <c r="M21">
+        <v>74.7</v>
+      </c>
+      <c r="N21" s="7">
+        <v>45650.499814814815</v>
+      </c>
+      <c r="O21" s="7">
+        <v>45650.499814814815</v>
+      </c>
+      <c r="P21" s="7">
+        <v>45650.499814814815</v>
+      </c>
+      <c r="Q21" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R21" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S21">
+        <v>23850</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1100381471</v>
+      </c>
+      <c r="B22">
+        <v>22241224387016</v>
+      </c>
+      <c r="C22">
+        <v>1300000074500620</v>
+      </c>
+      <c r="D22">
+        <v>2033033</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G22" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H22" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I22" t="s">
+        <v>1346</v>
+      </c>
+      <c r="K22">
+        <v>41690</v>
+      </c>
+      <c r="L22">
+        <v>25</v>
+      </c>
+      <c r="M22">
+        <v>93.15</v>
+      </c>
+      <c r="N22" s="7">
+        <v>45650.503020833334</v>
+      </c>
+      <c r="O22" s="7">
+        <v>45650.503020833334</v>
+      </c>
+      <c r="P22" s="7">
+        <v>45650.503020833334</v>
+      </c>
+      <c r="Q22" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R22" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S22">
+        <v>23850</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1100381471</v>
+      </c>
+      <c r="B23">
+        <v>22241224402716</v>
+      </c>
+      <c r="C23">
+        <v>1300000078746580</v>
+      </c>
+      <c r="D23">
+        <v>2163780</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1340</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H23" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I23" t="s">
+        <v>1346</v>
+      </c>
+      <c r="K23">
+        <v>41690</v>
+      </c>
+      <c r="L23">
+        <v>25</v>
+      </c>
+      <c r="M23">
+        <v>106.5</v>
+      </c>
+      <c r="N23" s="7">
+        <v>45650.510937500003</v>
+      </c>
+      <c r="O23" s="7">
+        <v>45650.510937500003</v>
+      </c>
+      <c r="P23" s="7">
+        <v>45650.510937500003</v>
+      </c>
+      <c r="Q23" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R23" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S23">
+        <v>23850</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1100381471</v>
+      </c>
+      <c r="B24">
+        <v>32241224372416</v>
+      </c>
+      <c r="C24">
+        <v>1100000055083660</v>
+      </c>
+      <c r="D24">
+        <v>1781843</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1340</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G24" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H24" t="s">
+        <v>1336</v>
+      </c>
+      <c r="I24" t="s">
+        <v>1347</v>
+      </c>
+      <c r="K24">
+        <v>41685</v>
+      </c>
+      <c r="L24">
+        <v>25</v>
+      </c>
+      <c r="M24">
+        <v>156.9</v>
+      </c>
+      <c r="N24" s="7">
+        <v>45650.460682870369</v>
+      </c>
+      <c r="O24" s="7">
+        <v>45650.460682870369</v>
+      </c>
+      <c r="P24" s="7">
+        <v>45650.460682870369</v>
+      </c>
+      <c r="Q24" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R24" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S24">
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1100381471</v>
+      </c>
+      <c r="B25">
+        <v>32241224377516</v>
+      </c>
+      <c r="C25">
+        <v>1100000056210220</v>
+      </c>
+      <c r="D25">
+        <v>1797973</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1340</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G25" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H25" t="s">
+        <v>1336</v>
+      </c>
+      <c r="I25" t="s">
+        <v>1347</v>
+      </c>
+      <c r="K25">
+        <v>41685</v>
+      </c>
+      <c r="L25">
+        <v>25</v>
+      </c>
+      <c r="M25">
+        <v>154.05000000000001</v>
+      </c>
+      <c r="N25" s="7">
+        <v>45650.463136574072</v>
+      </c>
+      <c r="O25" s="7">
+        <v>45650.463136574072</v>
+      </c>
+      <c r="P25" s="7">
+        <v>45650.463136574072</v>
+      </c>
+      <c r="Q25" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R25" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S25">
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1100381471</v>
+      </c>
+      <c r="B26">
+        <v>32241224398116</v>
+      </c>
+      <c r="C26">
+        <v>1900000071484640</v>
+      </c>
+      <c r="D26">
+        <v>5080469</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H26" t="s">
+        <v>1336</v>
+      </c>
+      <c r="I26" t="s">
+        <v>1349</v>
+      </c>
+      <c r="K26">
+        <v>39541</v>
+      </c>
+      <c r="L26">
+        <v>15</v>
+      </c>
+      <c r="M26">
+        <v>1149.05</v>
+      </c>
+      <c r="N26" s="7">
+        <v>45650.470879629633</v>
+      </c>
+      <c r="O26" s="7">
+        <v>45650.470891203702</v>
+      </c>
+      <c r="P26" s="7">
+        <v>45650.470891203702</v>
+      </c>
+      <c r="Q26" s="8">
+        <v>45686</v>
+      </c>
+      <c r="R26" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S26">
+        <v>51300</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1100381471</v>
+      </c>
+      <c r="B27">
+        <v>32241224447116</v>
+      </c>
+      <c r="C27">
+        <v>1100000066836810</v>
+      </c>
+      <c r="D27">
+        <v>1967594</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G27" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H27" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I27" t="s">
+        <v>1347</v>
+      </c>
+      <c r="K27">
+        <v>41685</v>
+      </c>
+      <c r="L27">
+        <v>25</v>
+      </c>
+      <c r="M27">
+        <v>150.35</v>
+      </c>
+      <c r="N27" s="7">
+        <v>45650.48741898148</v>
+      </c>
+      <c r="O27" s="7">
+        <v>45650.48741898148</v>
+      </c>
+      <c r="P27" s="7">
+        <v>45650.48741898148</v>
+      </c>
+      <c r="Q27" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R27" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S27">
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1100381471</v>
+      </c>
+      <c r="B28">
+        <v>32241224483916</v>
+      </c>
+      <c r="C28">
+        <v>1300000075122800</v>
+      </c>
+      <c r="D28">
+        <v>2052151</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1340</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G28" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H28" t="s">
+        <v>1336</v>
+      </c>
+      <c r="I28" t="s">
+        <v>1346</v>
+      </c>
+      <c r="K28">
+        <v>41690</v>
+      </c>
+      <c r="L28">
+        <v>25</v>
+      </c>
+      <c r="M28">
+        <v>93.4</v>
+      </c>
+      <c r="N28" s="7">
+        <v>45650.503958333335</v>
+      </c>
+      <c r="O28" s="7">
+        <v>45650.503958333335</v>
+      </c>
+      <c r="P28" s="7">
+        <v>45650.503958333335</v>
+      </c>
+      <c r="Q28" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R28" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S28">
+        <v>23850</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1100381471</v>
+      </c>
+      <c r="B29">
+        <v>32241224592316</v>
+      </c>
+      <c r="C29">
+        <v>1300000093193810</v>
+      </c>
+      <c r="D29">
+        <v>2527144</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G29" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H29" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I29" t="s">
+        <v>1346</v>
+      </c>
+      <c r="K29">
+        <v>41690</v>
+      </c>
+      <c r="L29">
+        <v>25</v>
+      </c>
+      <c r="M29">
+        <v>84.4</v>
+      </c>
+      <c r="N29" s="7">
+        <v>45650.534259259257</v>
+      </c>
+      <c r="O29" s="7">
+        <v>45650.534259259257</v>
+      </c>
+      <c r="P29" s="7">
+        <v>45650.534259259257</v>
+      </c>
+      <c r="Q29" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R29" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S29">
+        <v>23850</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1100381471</v>
+      </c>
+      <c r="B30">
+        <v>32241224594116</v>
+      </c>
+      <c r="C30">
+        <v>1300000093542270</v>
+      </c>
+      <c r="D30">
+        <v>2537359</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1340</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G30" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H30" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I30" t="s">
+        <v>1346</v>
+      </c>
+      <c r="K30">
+        <v>41690</v>
+      </c>
+      <c r="L30">
+        <v>25</v>
+      </c>
+      <c r="M30">
+        <v>88.6</v>
+      </c>
+      <c r="N30" s="7">
+        <v>45650.53496527778</v>
+      </c>
+      <c r="O30" s="7">
+        <v>45650.53496527778</v>
+      </c>
+      <c r="P30" s="7">
+        <v>45650.53496527778</v>
+      </c>
+      <c r="Q30" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R30" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S30">
+        <v>23850</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1100381471</v>
+      </c>
+      <c r="B31">
+        <v>32241224716216</v>
+      </c>
+      <c r="C31">
+        <v>1300000116016490</v>
+      </c>
+      <c r="D31">
+        <v>3029621</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G31" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H31" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I31" t="s">
+        <v>1346</v>
+      </c>
+      <c r="K31">
+        <v>41690</v>
+      </c>
+      <c r="L31">
+        <v>75</v>
+      </c>
+      <c r="M31">
+        <v>122.65</v>
+      </c>
+      <c r="N31" s="7">
+        <v>45650.584027777775</v>
+      </c>
+      <c r="O31" s="7">
+        <v>45650.584027777775</v>
+      </c>
+      <c r="P31" s="7">
+        <v>45650.584027777775</v>
+      </c>
+      <c r="Q31" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R31" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S31">
+        <v>23850</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1100381471</v>
+      </c>
+      <c r="B32">
+        <v>42241224212416</v>
+      </c>
+      <c r="C32">
+        <v>1300000026580020</v>
+      </c>
+      <c r="D32">
+        <v>626932</v>
+      </c>
+      <c r="E32" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G32" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H32" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I32" t="s">
+        <v>1346</v>
+      </c>
+      <c r="K32">
+        <v>41690</v>
+      </c>
+      <c r="L32">
+        <v>25</v>
+      </c>
+      <c r="M32">
+        <v>100.85</v>
+      </c>
+      <c r="N32" s="7">
+        <v>45650.419861111113</v>
+      </c>
+      <c r="O32" s="7">
+        <v>45650.419861111113</v>
+      </c>
+      <c r="P32" s="7">
+        <v>45650.419861111113</v>
+      </c>
+      <c r="Q32" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R32" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S32">
+        <v>23850</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1100381471</v>
+      </c>
+      <c r="B33">
+        <v>42241224257616</v>
+      </c>
+      <c r="C33">
+        <v>1400000043655850</v>
+      </c>
+      <c r="D33">
+        <v>1274376</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1340</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G33" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H33" t="s">
+        <v>1336</v>
+      </c>
+      <c r="I33" t="s">
+        <v>1350</v>
+      </c>
+      <c r="K33">
+        <v>41692</v>
+      </c>
+      <c r="L33">
+        <v>25</v>
+      </c>
+      <c r="M33">
+        <v>111.8</v>
+      </c>
+      <c r="N33" s="7">
+        <v>45650.428715277776</v>
+      </c>
+      <c r="O33" s="7">
+        <v>45650.428715277776</v>
+      </c>
+      <c r="P33" s="7">
+        <v>45650.428715277776</v>
+      </c>
+      <c r="Q33" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R33" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S33">
+        <v>23900</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1100381471</v>
+      </c>
+      <c r="B34">
+        <v>42241224435516</v>
+      </c>
+      <c r="C34">
+        <v>1900000075863830</v>
+      </c>
+      <c r="D34">
+        <v>5473089</v>
+      </c>
+      <c r="E34" t="s">
+        <v>1340</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G34" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H34" t="s">
+        <v>1336</v>
+      </c>
+      <c r="I34" t="s">
+        <v>1349</v>
+      </c>
+      <c r="K34">
+        <v>39541</v>
+      </c>
+      <c r="L34">
+        <v>15</v>
+      </c>
+      <c r="M34">
+        <v>1130.1500000000001</v>
+      </c>
+      <c r="N34" s="7">
+        <v>45650.479756944442</v>
+      </c>
+      <c r="O34" s="7">
+        <v>45650.479756944442</v>
+      </c>
+      <c r="P34" s="7">
+        <v>45650.479756944442</v>
+      </c>
+      <c r="Q34" s="8">
+        <v>45686</v>
+      </c>
+      <c r="R34" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S34">
+        <v>51300</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1100381471</v>
+      </c>
+      <c r="B35">
+        <v>42241224583716</v>
+      </c>
+      <c r="C35">
+        <v>1300000091060400</v>
+      </c>
+      <c r="D35">
+        <v>2462085</v>
+      </c>
+      <c r="E35" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G35" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H35" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I35" t="s">
+        <v>1346</v>
+      </c>
+      <c r="K35">
+        <v>41690</v>
+      </c>
+      <c r="L35">
+        <v>25</v>
+      </c>
+      <c r="M35">
+        <v>86.35</v>
+      </c>
+      <c r="N35" s="7">
+        <v>45650.530891203707</v>
+      </c>
+      <c r="O35" s="7">
+        <v>45650.530891203707</v>
+      </c>
+      <c r="P35" s="7">
+        <v>45650.530891203707</v>
+      </c>
+      <c r="Q35" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R35" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S35">
+        <v>23850</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1100381471</v>
+      </c>
+      <c r="B36">
+        <v>42241224601116</v>
+      </c>
+      <c r="C36">
+        <v>1200000132152250</v>
+      </c>
+      <c r="D36">
+        <v>4914258</v>
+      </c>
+      <c r="E36" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F36" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G36" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H36" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I36" t="s">
+        <v>1351</v>
+      </c>
+      <c r="K36">
+        <v>41687</v>
+      </c>
+      <c r="L36">
+        <v>25</v>
+      </c>
+      <c r="M36">
+        <v>83.05</v>
+      </c>
+      <c r="N36" s="7">
+        <v>45650.53565972222</v>
+      </c>
+      <c r="O36" s="7">
+        <v>45650.53565972222</v>
+      </c>
+      <c r="P36" s="7">
+        <v>45650.53565972222</v>
+      </c>
+      <c r="Q36" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R36" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S36">
+        <v>23800</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1100381471</v>
+      </c>
+      <c r="B37">
+        <v>42241224713516</v>
+      </c>
+      <c r="C37">
+        <v>1300000116231050</v>
+      </c>
+      <c r="D37">
+        <v>3030942</v>
+      </c>
+      <c r="E37" t="s">
+        <v>1340</v>
+      </c>
+      <c r="F37" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G37" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H37" t="s">
+        <v>1336</v>
+      </c>
+      <c r="I37" t="s">
+        <v>1346</v>
+      </c>
+      <c r="K37">
+        <v>41690</v>
+      </c>
+      <c r="L37">
+        <v>75</v>
+      </c>
+      <c r="M37">
+        <v>123.35</v>
+      </c>
+      <c r="N37" s="7">
+        <v>45650.584224537037</v>
+      </c>
+      <c r="O37" s="7">
+        <v>45650.584224537037</v>
+      </c>
+      <c r="P37" s="7">
+        <v>45650.584224537037</v>
+      </c>
+      <c r="Q37" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R37" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S37">
+        <v>23850</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1100381471</v>
+      </c>
+      <c r="B38">
+        <v>52241224313516</v>
+      </c>
+      <c r="C38">
+        <v>1100000057815240</v>
+      </c>
+      <c r="D38">
+        <v>1821060</v>
+      </c>
+      <c r="E38" t="s">
+        <v>1340</v>
+      </c>
+      <c r="F38" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G38" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H38" t="s">
+        <v>1336</v>
+      </c>
+      <c r="I38" t="s">
+        <v>1347</v>
+      </c>
+      <c r="K38">
+        <v>41685</v>
+      </c>
+      <c r="L38">
+        <v>25</v>
+      </c>
+      <c r="M38">
+        <v>147.4</v>
+      </c>
+      <c r="N38" s="7">
+        <v>45650.466979166667</v>
+      </c>
+      <c r="O38" s="7">
+        <v>45650.466979166667</v>
+      </c>
+      <c r="P38" s="7">
+        <v>45650.466979166667</v>
+      </c>
+      <c r="Q38" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R38" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S38">
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1100381471</v>
+      </c>
+      <c r="B39">
+        <v>52241224365016</v>
+      </c>
+      <c r="C39">
+        <v>1100000066978420</v>
+      </c>
+      <c r="D39">
+        <v>1969230</v>
+      </c>
+      <c r="E39" t="s">
+        <v>1340</v>
+      </c>
+      <c r="F39" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G39" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H39" t="s">
+        <v>1336</v>
+      </c>
+      <c r="I39" t="s">
+        <v>1347</v>
+      </c>
+      <c r="K39">
+        <v>41685</v>
+      </c>
+      <c r="L39">
+        <v>25</v>
+      </c>
+      <c r="M39">
+        <v>150.1</v>
+      </c>
+      <c r="N39" s="7">
+        <v>45650.487685185188</v>
+      </c>
+      <c r="O39" s="7">
+        <v>45650.487685185188</v>
+      </c>
+      <c r="P39" s="7">
+        <v>45650.487685185188</v>
+      </c>
+      <c r="Q39" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R39" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S39">
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1100381471</v>
+      </c>
+      <c r="B40">
+        <v>52241224387016</v>
+      </c>
+      <c r="C40">
+        <v>1300000072653780</v>
+      </c>
+      <c r="D40">
+        <v>1960237</v>
+      </c>
+      <c r="E40" t="s">
+        <v>1340</v>
+      </c>
+      <c r="F40" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G40" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H40" t="s">
+        <v>1336</v>
+      </c>
+      <c r="I40" t="s">
+        <v>1346</v>
+      </c>
+      <c r="K40">
+        <v>41690</v>
+      </c>
+      <c r="L40">
+        <v>50</v>
+      </c>
+      <c r="M40">
+        <v>79.75</v>
+      </c>
+      <c r="N40" s="7">
+        <v>45650.500254629631</v>
+      </c>
+      <c r="O40" s="7">
+        <v>45650.500254629631</v>
+      </c>
+      <c r="P40" s="7">
+        <v>45650.500254629631</v>
+      </c>
+      <c r="Q40" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R40" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S40">
+        <v>23850</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1100381471</v>
+      </c>
+      <c r="B41">
+        <v>52241224413416</v>
+      </c>
+      <c r="C41">
+        <v>1000000113403810</v>
+      </c>
+      <c r="D41">
+        <v>4450468</v>
+      </c>
+      <c r="E41" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F41" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G41" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H41" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I41" t="s">
+        <v>1348</v>
+      </c>
+      <c r="K41">
+        <v>35005</v>
+      </c>
+      <c r="L41">
+        <v>25</v>
+      </c>
+      <c r="M41">
+        <v>23775.4</v>
+      </c>
+      <c r="N41" s="7">
+        <v>45650.571203703701</v>
+      </c>
+      <c r="O41" s="7">
+        <v>45650.571203703701</v>
+      </c>
+      <c r="P41" s="7">
+        <v>45650.571203703701</v>
+      </c>
+      <c r="Q41" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R41" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S41">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1100381471</v>
+      </c>
+      <c r="B42">
+        <v>62241224198816</v>
+      </c>
+      <c r="C42">
+        <v>1400000040929170</v>
+      </c>
+      <c r="D42">
+        <v>1208083</v>
+      </c>
+      <c r="E42" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G42" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H42" t="s">
+        <v>1336</v>
+      </c>
+      <c r="I42" t="s">
+        <v>1350</v>
+      </c>
+      <c r="K42">
+        <v>41692</v>
+      </c>
+      <c r="L42">
+        <v>25</v>
+      </c>
+      <c r="M42">
+        <v>124</v>
+      </c>
+      <c r="N42" s="7">
+        <v>45650.42559027778</v>
+      </c>
+      <c r="O42" s="7">
+        <v>45650.42559027778</v>
+      </c>
+      <c r="P42" s="7">
+        <v>45650.42559027778</v>
+      </c>
+      <c r="Q42" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R42" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S42">
+        <v>23900</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1100381471</v>
+      </c>
+      <c r="B43">
+        <v>62241224316616</v>
+      </c>
+      <c r="C43">
+        <v>1100000054540860</v>
+      </c>
+      <c r="D43">
+        <v>1772779</v>
+      </c>
+      <c r="E43" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F43" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G43" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H43" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I43" t="s">
+        <v>1347</v>
+      </c>
+      <c r="K43">
+        <v>41685</v>
+      </c>
+      <c r="L43">
+        <v>25</v>
+      </c>
+      <c r="M43">
+        <v>157.55000000000001</v>
+      </c>
+      <c r="N43" s="7">
+        <v>45650.459780092591</v>
+      </c>
+      <c r="O43" s="7">
+        <v>45650.459780092591</v>
+      </c>
+      <c r="P43" s="7">
+        <v>45650.459780092591</v>
+      </c>
+      <c r="Q43" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R43" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S43">
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1100381471</v>
+      </c>
+      <c r="B44">
+        <v>102241224419416</v>
+      </c>
+      <c r="C44">
+        <v>1100000057644630</v>
+      </c>
+      <c r="D44">
+        <v>1818491</v>
+      </c>
+      <c r="E44" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F44" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G44" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H44" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I44" t="s">
+        <v>1347</v>
+      </c>
+      <c r="K44">
+        <v>41685</v>
+      </c>
+      <c r="L44">
+        <v>25</v>
+      </c>
+      <c r="M44">
+        <v>152.5</v>
+      </c>
+      <c r="N44" s="7">
+        <v>45650.466550925928</v>
+      </c>
+      <c r="O44" s="7">
+        <v>45650.466550925928</v>
+      </c>
+      <c r="P44" s="7">
+        <v>45650.466550925928</v>
+      </c>
+      <c r="Q44" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R44" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S44">
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1100381471</v>
+      </c>
+      <c r="B45">
+        <v>102241224483216</v>
+      </c>
+      <c r="C45">
+        <v>1100000067341590</v>
+      </c>
+      <c r="D45">
+        <v>1975114</v>
+      </c>
+      <c r="E45" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F45" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G45" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H45" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I45" t="s">
+        <v>1347</v>
+      </c>
+      <c r="K45">
+        <v>41685</v>
+      </c>
+      <c r="L45">
+        <v>25</v>
+      </c>
+      <c r="M45">
+        <v>145.55000000000001</v>
+      </c>
+      <c r="N45" s="7">
+        <v>45650.488668981481</v>
+      </c>
+      <c r="O45" s="7">
+        <v>45650.488668981481</v>
+      </c>
+      <c r="P45" s="7">
+        <v>45650.488668981481</v>
+      </c>
+      <c r="Q45" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R45" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S45">
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>1100381471</v>
+      </c>
+      <c r="B46">
+        <v>102241224619816</v>
+      </c>
+      <c r="C46">
+        <v>1200000133301410</v>
+      </c>
+      <c r="D46">
+        <v>4945124</v>
+      </c>
+      <c r="E46" t="s">
+        <v>1340</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G46" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H46" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I46" t="s">
+        <v>1351</v>
+      </c>
+      <c r="K46">
+        <v>41687</v>
+      </c>
+      <c r="L46">
+        <v>25</v>
+      </c>
+      <c r="M46">
+        <v>79.150000000000006</v>
+      </c>
+      <c r="N46" s="7">
+        <v>45650.537592592591</v>
+      </c>
+      <c r="O46" s="7">
+        <v>45650.537604166668</v>
+      </c>
+      <c r="P46" s="7">
+        <v>45650.537604166668</v>
+      </c>
+      <c r="Q46" s="8">
+        <v>45652</v>
+      </c>
+      <c r="R46" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S46">
+        <v>23800</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1100381471</v>
+      </c>
+      <c r="B47">
+        <v>28122412249143</v>
+      </c>
+      <c r="C47">
+        <v>435915326750681</v>
+      </c>
+      <c r="D47">
+        <v>150377844</v>
+      </c>
+      <c r="E47" t="s">
+        <v>1340</v>
+      </c>
+      <c r="G47" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H47" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I47" t="s">
+        <v>1352</v>
+      </c>
+      <c r="K47">
+        <v>441307</v>
+      </c>
+      <c r="L47">
+        <v>1</v>
+      </c>
+      <c r="M47">
+        <v>197.5</v>
+      </c>
+      <c r="N47" s="7">
+        <v>45650.728032407409</v>
+      </c>
+      <c r="O47" s="7">
+        <v>45650.728032407409</v>
+      </c>
+      <c r="P47" s="7">
+        <v>45650.728032407409</v>
+      </c>
+      <c r="Q47" s="8">
+        <v>45672</v>
+      </c>
+      <c r="R47" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S47">
+        <v>5900</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1100381471</v>
+      </c>
+      <c r="B48">
+        <v>38122412249693</v>
+      </c>
+      <c r="C48">
+        <v>435915326678868</v>
+      </c>
+      <c r="D48">
+        <v>150342813</v>
+      </c>
+      <c r="E48" t="s">
+        <v>1333</v>
+      </c>
+      <c r="G48" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H48" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I48" t="s">
+        <v>1352</v>
+      </c>
+      <c r="K48">
+        <v>441307</v>
+      </c>
+      <c r="L48">
+        <v>1</v>
+      </c>
+      <c r="M48">
+        <v>203.6</v>
+      </c>
+      <c r="N48" s="7">
+        <v>45650.70584490741</v>
+      </c>
+      <c r="O48" s="7">
+        <v>45650.70584490741</v>
+      </c>
+      <c r="P48" s="7">
+        <v>45650.70584490741</v>
+      </c>
+      <c r="Q48" s="8">
+        <v>45672</v>
+      </c>
+      <c r="R48" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S48">
+        <v>5900</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>1100381471</v>
+      </c>
+      <c r="B49">
+        <v>38122412252683</v>
+      </c>
+      <c r="C49">
+        <v>435915327387923</v>
+      </c>
+      <c r="D49">
+        <v>150437673</v>
+      </c>
+      <c r="E49" t="s">
+        <v>1340</v>
+      </c>
+      <c r="G49" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H49" t="s">
+        <v>1336</v>
+      </c>
+      <c r="I49" t="s">
+        <v>1353</v>
+      </c>
+      <c r="K49">
+        <v>441392</v>
+      </c>
+      <c r="L49">
+        <v>1</v>
+      </c>
+      <c r="M49">
+        <v>166.6</v>
+      </c>
+      <c r="N49" s="7">
+        <v>45650.743171296293</v>
+      </c>
+      <c r="O49" s="7">
+        <v>45650.743171296293</v>
+      </c>
+      <c r="P49" s="7">
+        <v>45650.743171296293</v>
+      </c>
+      <c r="Q49" s="8">
+        <v>45672</v>
+      </c>
+      <c r="R49" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S49">
+        <v>5950</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1100381471</v>
+      </c>
+      <c r="B50">
+        <v>38122412252683</v>
+      </c>
+      <c r="C50">
+        <v>435915327387923</v>
+      </c>
+      <c r="D50">
+        <v>150437675</v>
+      </c>
+      <c r="E50" t="s">
+        <v>1340</v>
+      </c>
+      <c r="G50" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H50" t="s">
+        <v>1336</v>
+      </c>
+      <c r="I50" t="s">
+        <v>1353</v>
+      </c>
+      <c r="K50">
+        <v>441392</v>
+      </c>
+      <c r="L50">
+        <v>1</v>
+      </c>
+      <c r="M50">
+        <v>166.5</v>
+      </c>
+      <c r="N50" s="7">
+        <v>45650.743171296293</v>
+      </c>
+      <c r="O50" s="7">
+        <v>45650.743171296293</v>
+      </c>
+      <c r="P50" s="7">
+        <v>45650.743171296293</v>
+      </c>
+      <c r="Q50" s="8">
+        <v>45672</v>
+      </c>
+      <c r="R50" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S50">
+        <v>5950</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>1100381471</v>
+      </c>
+      <c r="B51">
+        <v>48122412252613</v>
+      </c>
+      <c r="C51">
+        <v>435915327451316</v>
+      </c>
+      <c r="D51">
+        <v>150447435</v>
+      </c>
+      <c r="E51" t="s">
+        <v>1333</v>
+      </c>
+      <c r="G51" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H51" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I51" t="s">
+        <v>1354</v>
+      </c>
+      <c r="K51">
+        <v>441393</v>
+      </c>
+      <c r="L51">
+        <v>1</v>
+      </c>
+      <c r="M51">
+        <v>187.7</v>
+      </c>
+      <c r="N51" s="7">
+        <v>45650.745092592595</v>
+      </c>
+      <c r="O51" s="7">
+        <v>45650.745092592595</v>
+      </c>
+      <c r="P51" s="7">
+        <v>45650.745092592595</v>
+      </c>
+      <c r="Q51" s="8">
+        <v>45672</v>
+      </c>
+      <c r="R51" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S51">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1100381471</v>
+      </c>
+      <c r="B52">
+        <v>48122412252613</v>
+      </c>
+      <c r="C52">
+        <v>435915327451316</v>
+      </c>
+      <c r="D52">
+        <v>150447436</v>
+      </c>
+      <c r="E52" t="s">
+        <v>1333</v>
+      </c>
+      <c r="G52" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H52" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I52" t="s">
+        <v>1354</v>
+      </c>
+      <c r="K52">
+        <v>441393</v>
+      </c>
+      <c r="L52">
+        <v>1</v>
+      </c>
+      <c r="M52">
+        <v>187.7</v>
+      </c>
+      <c r="N52" s="7">
+        <v>45650.745092592595</v>
+      </c>
+      <c r="O52" s="7">
+        <v>45650.745092592595</v>
+      </c>
+      <c r="P52" s="7">
+        <v>45650.745092592595</v>
+      </c>
+      <c r="Q52" s="8">
+        <v>45672</v>
+      </c>
+      <c r="R52" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S52">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1100381471</v>
+      </c>
+      <c r="B53">
+        <v>68122412250253</v>
+      </c>
+      <c r="C53">
+        <v>435915327164307</v>
+      </c>
+      <c r="D53">
+        <v>150408843</v>
+      </c>
+      <c r="E53" t="s">
+        <v>1333</v>
+      </c>
+      <c r="G53" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H53" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I53" t="s">
+        <v>1353</v>
+      </c>
+      <c r="K53">
+        <v>441392</v>
+      </c>
+      <c r="L53">
+        <v>2</v>
+      </c>
+      <c r="M53">
+        <v>168.7</v>
+      </c>
+      <c r="N53" s="7">
+        <v>45650.735682870371</v>
+      </c>
+      <c r="O53" s="7">
+        <v>45650.735682870371</v>
+      </c>
+      <c r="P53" s="7">
+        <v>45650.735682870371</v>
+      </c>
+      <c r="Q53" s="8">
+        <v>45672</v>
+      </c>
+      <c r="R53" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S53">
+        <v>5950</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1100381471</v>
+      </c>
+      <c r="B54">
+        <v>68122412251013</v>
+      </c>
+      <c r="C54">
+        <v>435915327495933</v>
+      </c>
+      <c r="D54">
+        <v>150464791</v>
+      </c>
+      <c r="E54" t="s">
+        <v>1340</v>
+      </c>
+      <c r="G54" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H54" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I54" t="s">
+        <v>1354</v>
+      </c>
+      <c r="K54">
+        <v>441393</v>
+      </c>
+      <c r="L54">
+        <v>2</v>
+      </c>
+      <c r="M54">
+        <v>182.6</v>
+      </c>
+      <c r="N54" s="7">
+        <v>45650.749583333331</v>
+      </c>
+      <c r="O54" s="7">
+        <v>45650.749583333331</v>
+      </c>
+      <c r="P54" s="7">
+        <v>45650.749583333331</v>
+      </c>
+      <c r="Q54" s="8">
+        <v>45672</v>
+      </c>
+      <c r="R54" t="s">
+        <v>1339</v>
+      </c>
+      <c r="S54">
+        <v>6000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Brokerage Break Even Logic and Safe mode for Single Thread
</commit_message>
<xml_diff>
--- a/dhan_excel/DhanTrading.xlsx
+++ b/dhan_excel/DhanTrading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AlgoTrading\Books\Sucessful Algorithmic Trading\SucessfulAlgoTrading\dhan_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD14FA6-B40B-4E9F-9BD0-9F817CE3A281}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D973FA-0FD9-4E78-8BB0-ABE6C5BF631C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3F6F1494-9B09-4F57-8AEB-2BA84EF373A6}"/>
   </bookViews>
@@ -34,6 +34,7 @@
     <definedName name="ITM_TWO_KEY">Trade!$G$8</definedName>
     <definedName name="ITM_TWO_LTP">Trade!$H$8</definedName>
     <definedName name="Refresh">Trade!$B$29</definedName>
+    <definedName name="Safe_Mode">Trade!$B$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="1331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1491" uniqueCount="1340">
   <si>
     <t>Instrument</t>
   </si>
@@ -4010,9 +4011,6 @@
     <t>NIFTY-Dec2024-23600-CE</t>
   </si>
   <si>
-    <t>NIFTY CE</t>
-  </si>
-  <si>
     <t>BANKNIFTY-Jan2025-51700-PE</t>
   </si>
   <si>
@@ -4031,13 +4029,43 @@
     <t>BANKNIFTY-Jan2025-51200-CE</t>
   </si>
   <si>
-    <t>Buy Qty</t>
-  </si>
-  <si>
-    <t>Buy Price</t>
-  </si>
-  <si>
-    <t>L</t>
+    <t>Safe Mode</t>
+  </si>
+  <si>
+    <t>Transaction Charges</t>
+  </si>
+  <si>
+    <t>Stamp Duty</t>
+  </si>
+  <si>
+    <t>STT</t>
+  </si>
+  <si>
+    <t>SEBI Charges</t>
+  </si>
+  <si>
+    <t>IPFT</t>
+  </si>
+  <si>
+    <t>GST</t>
+  </si>
+  <si>
+    <t>Total Charges</t>
+  </si>
+  <si>
+    <t>BEP</t>
+  </si>
+  <si>
+    <t>Brokerage</t>
+  </si>
+  <si>
+    <t>PROFIT_TARGET_BEFORE_CHARGES</t>
+  </si>
+  <si>
+    <t>Profit Target after Charges</t>
+  </si>
+  <si>
+    <t>CRUDEOIL CE</t>
   </si>
 </sst>
 </file>
@@ -4093,7 +4121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -4109,6 +4137,7 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4423,11 +4452,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F7CD468-4C8C-49F2-898A-9AFC5D722CAC}">
-  <dimension ref="A1:Y35"/>
+  <dimension ref="A1:AK35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="12" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R16" sqref="R16"/>
+      <pane xSplit="12" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4436,8 +4465,8 @@
     <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="9.140625" customWidth="1"/>
     <col min="16" max="16" width="22.5703125" customWidth="1"/>
     <col min="17" max="17" width="10.7109375" customWidth="1"/>
@@ -4449,27 +4478,24 @@
     <col min="23" max="23" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="39" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="8"/>
-      <c r="F1">
-        <f>SUMIF(Orders!E:E,"BUY",Orders!L:L)</f>
-        <v>650</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1321</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4477,7 +4503,7 @@
         <v>23747.85</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -4547,13 +4573,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3">
         <f>IF(LEFT(B2,1)="N",25,IF(LEFT(B2,1)="B",15,IF(LEFT(B2,1)="C",100,"")))</f>
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>25</v>
@@ -4618,8 +4644,41 @@
       <c r="Y5" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA5" s="11" t="s">
+        <v>1336</v>
+      </c>
+      <c r="AB5" s="11" t="s">
+        <v>1328</v>
+      </c>
+      <c r="AC5" s="11" t="s">
+        <v>1329</v>
+      </c>
+      <c r="AD5" s="11" t="s">
+        <v>1330</v>
+      </c>
+      <c r="AE5" s="11" t="s">
+        <v>1331</v>
+      </c>
+      <c r="AF5" s="11" t="s">
+        <v>1332</v>
+      </c>
+      <c r="AG5" s="11" t="s">
+        <v>1333</v>
+      </c>
+      <c r="AH5" s="11" t="s">
+        <v>1334</v>
+      </c>
+      <c r="AI5" s="11" t="s">
+        <v>1335</v>
+      </c>
+      <c r="AJ5" s="11" t="s">
+        <v>1337</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="D6" s="10" t="s">
         <v>21</v>
       </c>
@@ -4629,14 +4688,14 @@
       </c>
       <c r="F6" s="10" t="str">
         <f>$B$22&amp;"_"&amp;E6</f>
-        <v>NIFTY_CE_23700</v>
-      </c>
-      <c r="G6" s="10">
+        <v>CRUDEOIL_CE_23700</v>
+      </c>
+      <c r="G6" s="10" t="e">
         <f>VLOOKUP(F6,OptionsLookUp!A:B,2,FALSE)</f>
-        <v>41683</v>
+        <v>#N/A</v>
       </c>
       <c r="H6" s="10">
-        <v>50.55</v>
+        <v>51.3</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>IF(I6&lt;&gt;"",ROUNDDOWN($B$7*(IF(AND(I6&gt;0,I6&lt;10),I6/10,1))/H6/$B$5,0)*$B$27,"")</f>
@@ -4646,11 +4705,11 @@
         <v>0</v>
       </c>
       <c r="L6" s="3" t="str">
-        <f>IF(O6&lt;&gt;"",(ATM_LTP-O6)*$B$5,"")</f>
+        <f>IF(O6&lt;&gt;"",(ATM_LTP-O6)*(J6*$B$5)/$B$27,"")</f>
         <v/>
       </c>
       <c r="S6" s="3" t="str">
-        <f>IF(O6&lt;&gt;"",ROUND(O6+(O6*$B$19),1),"")</f>
+        <f>IF(O6&lt;&gt;"",ROUND(O6*AK6,1),"")</f>
         <v/>
       </c>
       <c r="W6" s="3" t="str">
@@ -4658,15 +4717,59 @@
         <v/>
       </c>
       <c r="X6" s="3" t="str">
-        <f t="shared" ref="X6" si="0">IF(O6&lt;&gt;"",ROUND(O6+(O6*$B$17),1),"")</f>
+        <f>IF(O6&lt;&gt;"",ROUND(S6-(S6*B9),1),"")</f>
         <v/>
       </c>
       <c r="Y6" s="3" t="str">
         <f>IF(O6&lt;&gt;"",ROUND(O6-(O6*$B$18),1),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA6" t="str">
+        <f>IF(O6&lt;&gt;"",40,"")</f>
+        <v/>
+      </c>
+      <c r="AB6" t="str">
+        <f>IF(O6&lt;&gt;"",((O6+((O6*$B$8)+O6))*J6)*(0.0003503),"")</f>
+        <v/>
+      </c>
+      <c r="AC6" t="str">
+        <f>IF(O6&lt;&gt;"",(O6*J6*0.00003),"")</f>
+        <v/>
+      </c>
+      <c r="AD6" t="str">
+        <f>IF(O6&lt;&gt;"",(O6+(O6*$B$8))*J6*0.001,"")</f>
+        <v/>
+      </c>
+      <c r="AE6" t="str">
+        <f>IF(O6&lt;&gt;"",(O6+(O6+(O6*$B$8)))*J6*0.000001,"")</f>
+        <v/>
+      </c>
+      <c r="AF6" t="str">
+        <f>IF(O6&lt;&gt;"",(O6+(O6+(O6*$B$8)))*J6*0.000005,"")</f>
+        <v/>
+      </c>
+      <c r="AG6" t="str">
+        <f>IF(O6&lt;&gt;"",(AA6+AB6+AE6)*0.18,"")</f>
+        <v/>
+      </c>
+      <c r="AH6" t="str">
+        <f>IF(O6&lt;&gt;"",SUM(AA6:AG6),"")</f>
+        <v/>
+      </c>
+      <c r="AI6" t="str">
+        <f>IF(O6&lt;&gt;"",AH6/J6,"")</f>
+        <v/>
+      </c>
+      <c r="AJ6" t="str">
+        <f>IF(O6&lt;&gt;"",O6+(O6*B8),"")</f>
+        <v/>
+      </c>
+      <c r="AK6" t="str">
+        <f>IF(O6&lt;&gt;"",(AJ6+AI6)/O6,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -4681,33 +4784,33 @@
         <v>23650</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" ref="F7:F9" si="1">$B$22&amp;"_"&amp;E7</f>
-        <v>NIFTY_CE_23650</v>
-      </c>
-      <c r="G7">
+        <f t="shared" ref="F7:F9" si="0">$B$22&amp;"_"&amp;E7</f>
+        <v>CRUDEOIL_CE_23650</v>
+      </c>
+      <c r="G7" t="e">
         <f>VLOOKUP(F7,OptionsLookUp!A:B,2,FALSE)</f>
-        <v>41681</v>
+        <v>#N/A</v>
       </c>
       <c r="H7">
-        <v>100.65</v>
+        <v>100.2</v>
       </c>
       <c r="J7" s="3" t="str">
-        <f t="shared" ref="J7:J9" si="2">IF(I7&lt;&gt;"",ROUNDDOWN($B$7*(IF(AND(I7&gt;0,I7&lt;10),I7/10,1))/H7/$B$5,0)*$B$27,"")</f>
+        <f t="shared" ref="J7:J9" si="1">IF(I7&lt;&gt;"",ROUNDDOWN($B$7*(IF(AND(I7&gt;0,I7&lt;10),I7/10,1))/H7/$B$5,0)*$B$27,"")</f>
         <v/>
       </c>
       <c r="K7" t="b">
         <v>0</v>
       </c>
       <c r="L7" s="3" t="str">
-        <f>IF(O7&lt;&gt;"",(ITM_ONE_LTP-O7)*$B$5,"")</f>
+        <f>IF(O7&lt;&gt;"",(ITM_ONE_LTP-O7)*(J7*$B$5)/$B$27,"")</f>
         <v/>
       </c>
       <c r="S7" s="3" t="str">
-        <f t="shared" ref="S7:S9" si="3">IF(O7&lt;&gt;"",ROUND(O7+(O7*$B$19),1),"")</f>
+        <f t="shared" ref="S7:S9" si="2">IF(O7&lt;&gt;"",ROUND(O7+(O7*$B$19),1),"")</f>
         <v/>
       </c>
       <c r="W7" s="3" t="str">
-        <f t="shared" ref="W7:W9" si="4">IF(O7&lt;&gt;"",ROUND(O7-(O7*$B$20),1),"")</f>
+        <f t="shared" ref="W7:W9" si="3">IF(O7&lt;&gt;"",ROUND(O7-(O7*$B$20),1),"")</f>
         <v/>
       </c>
       <c r="X7" s="3" t="str">
@@ -4715,11 +4818,55 @@
         <v/>
       </c>
       <c r="Y7" s="3" t="str">
-        <f t="shared" ref="Y7:Y9" si="5">IF(O7&lt;&gt;"",ROUND(O7-(O7*$B$18),1),"")</f>
+        <f t="shared" ref="Y7:Y9" si="4">IF(O7&lt;&gt;"",ROUND(O7-(O7*$B$18),1),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA7" s="11" t="str">
+        <f t="shared" ref="AA7:AA9" si="5">IF(O7&lt;&gt;"",40,"")</f>
+        <v/>
+      </c>
+      <c r="AB7" s="11" t="str">
+        <f t="shared" ref="AB7:AB9" si="6">IF(O7&lt;&gt;"",((O7+((O7*$B$8)+O7))*J7)*(0.0003503),"")</f>
+        <v/>
+      </c>
+      <c r="AC7" s="11" t="str">
+        <f t="shared" ref="AC7:AC9" si="7">IF(O7&lt;&gt;"",(O7*J7*0.00003),"")</f>
+        <v/>
+      </c>
+      <c r="AD7" s="11" t="str">
+        <f t="shared" ref="AD7:AD9" si="8">IF(O7&lt;&gt;"",(O7+(O7*$B$8))*J7*0.001,"")</f>
+        <v/>
+      </c>
+      <c r="AE7" s="11" t="str">
+        <f t="shared" ref="AE7:AE9" si="9">IF(O7&lt;&gt;"",(O7+(O7+(O7*$B$8)))*J7*0.000001,"")</f>
+        <v/>
+      </c>
+      <c r="AF7" s="11" t="str">
+        <f t="shared" ref="AF7:AF9" si="10">IF(O7&lt;&gt;"",(O7+(O7+(O7*$B$8)))*J7*0.000005,"")</f>
+        <v/>
+      </c>
+      <c r="AG7" s="11" t="str">
+        <f t="shared" ref="AG7:AG9" si="11">IF(O7&lt;&gt;"",(AA7+AB7+AE7)*0.18,"")</f>
+        <v/>
+      </c>
+      <c r="AH7" s="11" t="str">
+        <f t="shared" ref="AH7:AH9" si="12">IF(O7&lt;&gt;"",SUM(AA7:AG7),"")</f>
+        <v/>
+      </c>
+      <c r="AI7" s="11" t="str">
+        <f t="shared" ref="AI7:AI9" si="13">IF(O7&lt;&gt;"",AH7/J7,"")</f>
+        <v/>
+      </c>
+      <c r="AJ7" s="11" t="str">
+        <f t="shared" ref="AJ7:AJ9" si="14">IF(O7&lt;&gt;"",O7+(O7*B9),"")</f>
+        <v/>
+      </c>
+      <c r="AK7" s="11" t="str">
+        <f t="shared" ref="AK7:AK9" si="15">IF(O7&lt;&gt;"",(AJ7+AI7)/O7,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -4734,45 +4881,89 @@
         <v>23600</v>
       </c>
       <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>CRUDEOIL_CE_23600</v>
+      </c>
+      <c r="G8" t="e">
+        <f>VLOOKUP(F8,OptionsLookUp!A:B,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H8">
+        <v>150</v>
+      </c>
+      <c r="J8" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>NIFTY_CE_23600</v>
-      </c>
-      <c r="G8">
-        <f>VLOOKUP(F8,OptionsLookUp!A:B,2,FALSE)</f>
-        <v>41672</v>
-      </c>
-      <c r="H8">
-        <v>150.55000000000001</v>
-      </c>
-      <c r="J8" s="3" t="str">
+        <v/>
+      </c>
+      <c r="K8" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3" t="str">
+        <f>IF(O8&lt;&gt;"",(ITM_TWO_LTP-O8)*(J8*$B$5)/$B$27,"")</f>
+        <v/>
+      </c>
+      <c r="S8" s="3" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K8" t="b">
-        <v>0</v>
-      </c>
-      <c r="L8" s="3" t="str">
-        <f>IF(O8&lt;&gt;"",(ITM_TWO_LTP-O8)*$B$5,"")</f>
-        <v/>
-      </c>
-      <c r="S8" s="3" t="str">
+      <c r="W8" s="3" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W8" s="3" t="str">
+      <c r="X8" s="3" t="str">
+        <f t="shared" ref="X8:X9" si="16">IF(O8&lt;&gt;"",ROUND(O8+(O8*$B$17),1),"")</f>
+        <v/>
+      </c>
+      <c r="Y8" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X8" s="3" t="str">
-        <f t="shared" ref="X8:X9" si="6">IF(O8&lt;&gt;"",ROUND(O8+(O8*$B$17),1),"")</f>
-        <v/>
-      </c>
-      <c r="Y8" s="3" t="str">
+      <c r="AA8" s="11" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AB8" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AC8" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AD8" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AE8" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AF8" s="11" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="AG8" s="11" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AH8" s="11" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="AI8" s="11" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="AJ8" s="11" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="AK8" s="11" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -4787,45 +4978,89 @@
         <v>23550</v>
       </c>
       <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>CRUDEOIL_CE_23550</v>
+      </c>
+      <c r="G9" t="e">
+        <f>VLOOKUP(F9,OptionsLookUp!A:B,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H9">
+        <v>200.5</v>
+      </c>
+      <c r="J9" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>NIFTY_CE_23550</v>
-      </c>
-      <c r="G9">
-        <f>VLOOKUP(F9,OptionsLookUp!A:B,2,FALSE)</f>
-        <v>41665</v>
-      </c>
-      <c r="H9">
-        <v>200.1</v>
-      </c>
-      <c r="J9" s="3" t="str">
+        <v/>
+      </c>
+      <c r="K9" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3" t="str">
+        <f>IF(O9&lt;&gt;"",(ITM_THREE_LTP-O9)*(J9*$B$5)/$B$27,"")</f>
+        <v/>
+      </c>
+      <c r="S9" s="3" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K9" t="b">
-        <v>0</v>
-      </c>
-      <c r="L9" s="3" t="str">
-        <f>IF(O9&lt;&gt;"",(ITM_THREE_LTP-O9)*$B$5,"")</f>
-        <v/>
-      </c>
-      <c r="S9" s="3" t="str">
+      <c r="W9" s="3" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W9" s="3" t="str">
+      <c r="X9" s="3" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="Y9" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X9" s="3" t="str">
+      <c r="AA9" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AB9" s="11" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="Y9" s="3" t="str">
-        <f t="shared" si="5"/>
+      <c r="AC9" s="11" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AD9" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AE9" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AF9" s="11" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="AG9" s="11" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AH9" s="11" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="AI9" s="11" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="AJ9" s="11" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="AK9" s="11" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -4834,15 +5069,15 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>1323</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -4866,15 +5101,15 @@
         <v>23550</v>
       </c>
       <c r="J13" t="s">
+        <v>1323</v>
+      </c>
+      <c r="K13" t="s">
         <v>1324</v>
-      </c>
-      <c r="K13" t="s">
-        <v>1325</v>
       </c>
       <c r="R13" s="9"/>
       <c r="S13" s="6"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -4886,19 +5121,19 @@
       </c>
       <c r="F14">
         <f>ROUND((($B$7*E14)/$H$6)/$B$5,0)</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G14">
         <f>ROUND((($B$7*E14)/$H$7)/$B$5,0)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <f>ROUND((($B$7*E14)/$H$8)/$B$5,0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I14">
         <f>ROUND((($B$7*E14)/$H$9)/$B$5,0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J14">
         <f>E14*$B$13*$B$7*$B$8</f>
@@ -4910,37 +5145,37 @@
       </c>
       <c r="R14" s="9"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="E15" s="1">
         <v>0.2</v>
       </c>
       <c r="F15">
-        <f t="shared" ref="F15:F23" si="7">ROUND((($B$7*E15)/$H$6)/$B$5,0)</f>
-        <v>16</v>
+        <f t="shared" ref="F15:F23" si="17">ROUND((($B$7*E15)/$H$6)/$B$5,0)</f>
+        <v>4</v>
       </c>
       <c r="G15">
-        <f t="shared" ref="G15:G23" si="8">ROUND((($B$7*E15)/$H$7)/$B$5,0)</f>
-        <v>8</v>
+        <f t="shared" ref="G15:G23" si="18">ROUND((($B$7*E15)/$H$7)/$B$5,0)</f>
+        <v>2</v>
       </c>
       <c r="H15">
-        <f t="shared" ref="H15:H23" si="9">ROUND((($B$7*E15)/$H$8)/$B$5,0)</f>
-        <v>5</v>
+        <f t="shared" ref="H15:H23" si="19">ROUND((($B$7*E15)/$H$8)/$B$5,0)</f>
+        <v>1</v>
       </c>
       <c r="I15">
-        <f t="shared" ref="I15:I23" si="10">ROUND((($B$7*E15)/$H$9)/$B$5,0)</f>
-        <v>4</v>
+        <f t="shared" ref="I15:I23" si="20">ROUND((($B$7*E15)/$H$9)/$B$5,0)</f>
+        <v>1</v>
       </c>
       <c r="J15">
-        <f t="shared" ref="J15:J23" si="11">E15*$B$13*$B$7*$B$8</f>
+        <f t="shared" ref="J15:J23" si="21">E15*$B$13*$B$7*$B$8</f>
         <v>400</v>
       </c>
       <c r="K15">
-        <f t="shared" ref="K15:K23" si="12">E15*$B$14*$B$8*$B$7</f>
+        <f t="shared" ref="K15:K23" si="22">E15*$B$14*$B$8*$B$7</f>
         <v>1200.0000000000002</v>
       </c>
       <c r="R15" s="9"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
@@ -4948,32 +5183,32 @@
         <v>0.3</v>
       </c>
       <c r="F16">
-        <f t="shared" si="7"/>
-        <v>24</v>
+        <f t="shared" si="17"/>
+        <v>6</v>
       </c>
       <c r="G16">
-        <f t="shared" si="8"/>
-        <v>12</v>
+        <f t="shared" si="18"/>
+        <v>3</v>
       </c>
       <c r="H16">
-        <f t="shared" si="9"/>
-        <v>8</v>
+        <f t="shared" si="19"/>
+        <v>2</v>
       </c>
       <c r="I16">
-        <f t="shared" si="10"/>
-        <v>6</v>
+        <f t="shared" si="20"/>
+        <v>1</v>
       </c>
       <c r="J16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v>600</v>
       </c>
       <c r="K16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="22"/>
         <v>1799.9999999999998</v>
       </c>
       <c r="R16" s="9"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -4985,32 +5220,32 @@
         <v>0.4</v>
       </c>
       <c r="F17">
-        <f t="shared" si="7"/>
-        <v>32</v>
+        <f t="shared" si="17"/>
+        <v>8</v>
       </c>
       <c r="G17">
-        <f t="shared" si="8"/>
-        <v>16</v>
+        <f t="shared" si="18"/>
+        <v>4</v>
       </c>
       <c r="H17">
-        <f t="shared" si="9"/>
-        <v>11</v>
+        <f t="shared" si="19"/>
+        <v>3</v>
       </c>
       <c r="I17">
-        <f t="shared" si="10"/>
-        <v>8</v>
+        <f t="shared" si="20"/>
+        <v>2</v>
       </c>
       <c r="J17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v>800</v>
       </c>
       <c r="K17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="22"/>
         <v>2400.0000000000005</v>
       </c>
       <c r="R17" s="9"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -5022,32 +5257,32 @@
         <v>0.5</v>
       </c>
       <c r="F18">
-        <f t="shared" si="7"/>
-        <v>40</v>
+        <f t="shared" si="17"/>
+        <v>10</v>
       </c>
       <c r="G18">
-        <f t="shared" si="8"/>
-        <v>20</v>
+        <f t="shared" si="18"/>
+        <v>5</v>
       </c>
       <c r="H18">
-        <f t="shared" si="9"/>
-        <v>13</v>
+        <f t="shared" si="19"/>
+        <v>3</v>
       </c>
       <c r="I18">
-        <f t="shared" si="10"/>
-        <v>10</v>
+        <f t="shared" si="20"/>
+        <v>2</v>
       </c>
       <c r="J18">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v>1000</v>
       </c>
       <c r="K18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="22"/>
         <v>3000</v>
       </c>
       <c r="R18" s="9"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -5059,32 +5294,32 @@
         <v>0.6</v>
       </c>
       <c r="F19">
-        <f t="shared" si="7"/>
-        <v>47</v>
+        <f t="shared" si="17"/>
+        <v>12</v>
       </c>
       <c r="G19">
-        <f t="shared" si="8"/>
-        <v>24</v>
+        <f t="shared" si="18"/>
+        <v>6</v>
       </c>
       <c r="H19">
-        <f t="shared" si="9"/>
-        <v>16</v>
+        <f t="shared" si="19"/>
+        <v>4</v>
       </c>
       <c r="I19">
-        <f t="shared" si="10"/>
-        <v>12</v>
+        <f t="shared" si="20"/>
+        <v>3</v>
       </c>
       <c r="J19">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v>1200</v>
       </c>
       <c r="K19">
-        <f t="shared" si="12"/>
+        <f t="shared" si="22"/>
         <v>3599.9999999999995</v>
       </c>
       <c r="R19" s="9"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -5096,142 +5331,136 @@
         <v>0.7</v>
       </c>
       <c r="F20">
-        <f t="shared" si="7"/>
-        <v>55</v>
+        <f t="shared" si="17"/>
+        <v>14</v>
       </c>
       <c r="G20">
-        <f t="shared" si="8"/>
-        <v>28</v>
+        <f t="shared" si="18"/>
+        <v>7</v>
       </c>
       <c r="H20">
-        <f t="shared" si="9"/>
-        <v>19</v>
+        <f t="shared" si="19"/>
+        <v>5</v>
       </c>
       <c r="I20">
-        <f t="shared" si="10"/>
-        <v>14</v>
+        <f t="shared" si="20"/>
+        <v>3</v>
       </c>
       <c r="J20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v>1400</v>
       </c>
       <c r="K20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="22"/>
         <v>4200</v>
       </c>
       <c r="R20" s="9"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E21" s="1">
         <v>0.8</v>
       </c>
       <c r="F21">
-        <f t="shared" si="7"/>
-        <v>63</v>
+        <f t="shared" si="17"/>
+        <v>16</v>
       </c>
       <c r="G21">
-        <f t="shared" si="8"/>
-        <v>32</v>
+        <f t="shared" si="18"/>
+        <v>8</v>
       </c>
       <c r="H21">
-        <f t="shared" si="9"/>
-        <v>21</v>
+        <f t="shared" si="19"/>
+        <v>5</v>
       </c>
       <c r="I21">
-        <f t="shared" si="10"/>
-        <v>16</v>
+        <f t="shared" si="20"/>
+        <v>4</v>
       </c>
       <c r="J21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v>1600</v>
       </c>
       <c r="K21">
-        <f t="shared" si="12"/>
+        <f t="shared" si="22"/>
         <v>4800.0000000000009</v>
       </c>
       <c r="R21" s="9"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B22" t="str">
         <f>B23&amp;"_"&amp;B24</f>
-        <v>NIFTY_CE</v>
+        <v>CRUDEOIL_CE</v>
       </c>
       <c r="E22" s="1">
         <v>0.9</v>
       </c>
       <c r="F22">
-        <f t="shared" si="7"/>
-        <v>71</v>
+        <f t="shared" si="17"/>
+        <v>18</v>
       </c>
       <c r="G22">
-        <f t="shared" si="8"/>
-        <v>36</v>
+        <f t="shared" si="18"/>
+        <v>9</v>
       </c>
       <c r="H22">
-        <f t="shared" si="9"/>
-        <v>24</v>
+        <f t="shared" si="19"/>
+        <v>6</v>
       </c>
       <c r="I22">
-        <f t="shared" si="10"/>
-        <v>18</v>
+        <f t="shared" si="20"/>
+        <v>4</v>
       </c>
       <c r="J22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v>1800</v>
       </c>
       <c r="K22">
-        <f t="shared" si="12"/>
+        <f t="shared" si="22"/>
         <v>5400.0000000000009</v>
       </c>
       <c r="R22" s="9"/>
-      <c r="S22" t="s">
-        <v>1330</v>
-      </c>
-      <c r="T22" t="s">
-        <v>1330</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
       <c r="B23" t="str">
         <f>LEFT(B2,FIND(" ",B2,1)-1)</f>
-        <v>NIFTY</v>
+        <v>CRUDEOIL</v>
       </c>
       <c r="E23" s="1">
         <v>1</v>
       </c>
       <c r="F23">
-        <f t="shared" si="7"/>
-        <v>79</v>
+        <f t="shared" si="17"/>
+        <v>19</v>
       </c>
       <c r="G23">
-        <f t="shared" si="8"/>
-        <v>40</v>
+        <f t="shared" si="18"/>
+        <v>10</v>
       </c>
       <c r="H23">
-        <f t="shared" si="9"/>
-        <v>27</v>
+        <f t="shared" si="19"/>
+        <v>7</v>
       </c>
       <c r="I23">
-        <f t="shared" si="10"/>
-        <v>20</v>
+        <f t="shared" si="20"/>
+        <v>5</v>
       </c>
       <c r="J23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v>2000</v>
       </c>
       <c r="K23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="22"/>
         <v>6000</v>
       </c>
       <c r="R23" s="9"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -5240,36 +5469,36 @@
         <v>CE</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>54</v>
       </c>
       <c r="B25">
         <f>VLOOKUP(B23,IndexLookup!A1:B4,2,FALSE)</f>
-        <v>13</v>
+        <v>436953</v>
       </c>
       <c r="E25" s="9"/>
       <c r="G25" s="9"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E26" s="9"/>
       <c r="G26" s="9"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>18</v>
       </c>
       <c r="B27">
         <f>IF(OR(LEFT(B2,1)="N",LEFT(B2,1)="B"),B5,1)</f>
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E27" s="9"/>
       <c r="G27" s="9"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E28" s="9"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>1291</v>
       </c>
@@ -5278,11 +5507,11 @@
       </c>
       <c r="E29" s="9"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E30" s="9"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>1292</v>
       </c>
       <c r="B31" t="b">
@@ -5290,23 +5519,19 @@
       </c>
       <c r="E31" s="9"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E32" s="9"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>1328</v>
-      </c>
-      <c r="B33">
-        <f>SUMIF(Orders!E:E,"BUY",Orders!L:L)</f>
-        <v>650</v>
+      <c r="A33" s="4" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B33" s="11" t="b">
+        <v>0</v>
       </c>
       <c r="E33" s="9"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>1329</v>
-      </c>
       <c r="E34" s="9"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -5323,7 +5548,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B29" xr:uid="{A1FEE6D5-54C4-461C-B04B-7F0563CB22A3}">
       <formula1>"True, False"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31" xr:uid="{AABBCC32-78FC-4E10-AEEC-401979DA1033}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31 B33" xr:uid="{AABBCC32-78FC-4E10-AEEC-401979DA1033}">
       <formula1>"FALSE,TRUE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -15424,7 +15649,7 @@
         <v>1313</v>
       </c>
       <c r="I2" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="K2">
         <v>39550</v>
@@ -15480,7 +15705,7 @@
         <v>1313</v>
       </c>
       <c r="I3" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="K3">
         <v>39550</v>
@@ -15536,7 +15761,7 @@
         <v>1318</v>
       </c>
       <c r="I4" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="K4">
         <v>39550</v>
@@ -15760,7 +15985,7 @@
         <v>1318</v>
       </c>
       <c r="I8" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K8">
         <v>41681</v>
@@ -15984,7 +16209,7 @@
         <v>1318</v>
       </c>
       <c r="I12" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="K12">
         <v>39536</v>
@@ -16040,7 +16265,7 @@
         <v>1318</v>
       </c>
       <c r="I13" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="K13">
         <v>39536</v>
@@ -16096,7 +16321,7 @@
         <v>1318</v>
       </c>
       <c r="I14" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="K14">
         <v>39536</v>
@@ -16376,7 +16601,7 @@
         <v>1318</v>
       </c>
       <c r="I19" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K19">
         <v>41681</v>
@@ -16432,7 +16657,7 @@
         <v>1313</v>
       </c>
       <c r="I20" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="K20">
         <v>39550</v>
@@ -16600,7 +16825,7 @@
         <v>1318</v>
       </c>
       <c r="I23" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="K23">
         <v>39536</v>
@@ -16656,7 +16881,7 @@
         <v>1318</v>
       </c>
       <c r="I24" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="K24">
         <v>39536</v>
@@ -16712,7 +16937,7 @@
         <v>1318</v>
       </c>
       <c r="I25" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="K25">
         <v>39536</v>

</xml_diff>